<commit_message>
todo update and infowindow's message style changed
</commit_message>
<xml_diff>
--- a/src/main/resources/TODOs.xlsx
+++ b/src/main/resources/TODOs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace\incident-app\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE361FC-7A80-42CF-8A03-F4C43944A17D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601F5189-F976-46A3-9710-CA9C8A5B9FC9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9972" windowHeight="8244" activeTab="2" xr2:uid="{AA738D5C-D5BE-4907-AFCA-ACBAF9B3F897}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -164,9 +164,6 @@
     <t>When reporting new incident +2 infowindows open they don't close</t>
   </si>
   <si>
-    <t>current location spotted with the user photo or icon</t>
-  </si>
-  <si>
     <t>set timeout in js (in 10.000 miliseconds send 10 requests)</t>
   </si>
   <si>
@@ -188,7 +185,10 @@
     <t>see the application on mobile(IE)</t>
   </si>
   <si>
-    <t>CLOSED</t>
+    <t>current location spotted with the user icon</t>
+  </si>
+  <si>
+    <t>user should report an incident on his current location</t>
   </si>
 </sst>
 </file>
@@ -220,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,12 +242,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -303,9 +297,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,14 +306,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="286">
+  <dxfs count="151">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -435,6 +423,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -535,23 +533,104 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <color theme="9" tint="-0.24994659260841701"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -750,91 +829,96 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <color theme="9" tint="-0.24994659260841701"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -847,82 +931,6 @@
         <i val="0"/>
         <color theme="9" tint="-0.24994659260841701"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -935,6 +943,72 @@
         <i val="0"/>
         <color theme="9" tint="-0.24994659260841701"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -947,92 +1021,6 @@
         <i val="0"/>
         <color theme="9" tint="-0.24994659260841701"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -1046,46 +1034,8 @@
         <color theme="9" tint="-0.24994659260841701"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1095,1202 +1045,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC7A1E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF7030A0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8CCF5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2943,8 +1698,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFCC"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFFFFFCC"/>
       <color rgb="FFF8CCF5"/>
       <color rgb="FFF9B9F4"/>
       <color rgb="FFC7A1E3"/>
@@ -3539,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466B8D82-E7DF-4CF4-AFC0-ECEA7696B0DD}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3772,23 +2527,23 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+    <row r="13" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -3808,23 +2563,23 @@
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
+    <row r="15" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="18"/>
+      <c r="E15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -3844,23 +2599,23 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17">
+    <row r="17" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
         <v>16</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="18"/>
+      <c r="E17" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -3875,161 +2630,171 @@
       <c r="D18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15">
+    <row r="19" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
         <v>18</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="23" t="s">
+      <c r="C19" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="23"/>
+      <c r="E19" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="18" t="s">
+      <c r="C20" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="16"/>
+      <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>21</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D22" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="16"/>
+      <c r="E22" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="18" t="s">
+      <c r="C23" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="16"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="18" t="s">
+      <c r="C24" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="18" t="s">
+      <c r="C25" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="16"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="18" t="s">
+      <c r="C26" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="16"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -4459,459 +3224,506 @@
   </sheetData>
   <autoFilter ref="A1:F15" xr:uid="{8ACA0151-78CB-428A-BBDA-F3EEE46416DA}"/>
   <conditionalFormatting sqref="A2:F12">
-    <cfRule type="containsText" dxfId="285" priority="133" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="150" priority="146" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="284" priority="134" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="149" priority="147" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="283" priority="135" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="148" priority="148" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="136" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="147" priority="149" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="281" priority="137" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="146" priority="150" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="280" priority="138" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="145" priority="151" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="279" priority="139" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="144" priority="152" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="278" priority="140" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="143" priority="153" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="141" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="142" priority="154" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="276" priority="122" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="141" priority="135" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="275" priority="123" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="140" priority="136" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="274" priority="124" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="139" priority="137" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="125" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="138" priority="138" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="272" priority="126" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="137" priority="139" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="271" priority="127" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="136" priority="140" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="128" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="135" priority="141" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="129" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="134" priority="142" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="268" priority="130" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="133" priority="143" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="267" priority="131" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="132" priority="144" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="266" priority="112" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="131" priority="125" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="113" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="130" priority="126" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="264" priority="114" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="129" priority="127" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="263" priority="115" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="128" priority="128" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="116" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="127" priority="129" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="117" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="126" priority="130" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="260" priority="118" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="125" priority="131" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="259" priority="119" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="124" priority="132" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="120" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="123" priority="133" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="121" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="122" priority="134" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="256" priority="102" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="121" priority="115" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="255" priority="103" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="120" priority="116" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="254" priority="104" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="119" priority="117" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="253" priority="105" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="118" priority="118" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="252" priority="106" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="117" priority="119" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="251" priority="107" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="116" priority="120" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="108" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="115" priority="121" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="109" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="114" priority="122" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="248" priority="110" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="113" priority="123" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="247" priority="111" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="112" priority="124" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="246" priority="67" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="111" priority="80" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="92" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="110" priority="105" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="244" priority="93" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="109" priority="106" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="243" priority="94" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="108" priority="107" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="242" priority="95" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="107" priority="108" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="96" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="106" priority="109" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="240" priority="97" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="105" priority="110" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="239" priority="98" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="104" priority="111" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="99" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="103" priority="112" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="100" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="102" priority="113" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="236" priority="101" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="101" priority="114" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="containsText" dxfId="235" priority="71" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="100" priority="84" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="82" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="99" priority="95" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="83" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="98" priority="96" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="232" priority="84" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="97" priority="97" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="231" priority="85" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="96" priority="98" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="86" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="95" priority="99" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="87" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="94" priority="100" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="228" priority="88" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="93" priority="101" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="227" priority="89" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="92" priority="102" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="90" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="91" priority="103" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="91" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="90" priority="104" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="containsText" dxfId="224" priority="72" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="89" priority="85" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="223" priority="73" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="88" priority="86" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="74" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="87" priority="87" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="75" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="86" priority="88" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="76" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="219" priority="77" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="84" priority="90" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="78" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="83" priority="91" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="79" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="82" priority="92" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="216" priority="80" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="81" priority="93" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="215" priority="81" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="80" priority="94" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F80">
-    <cfRule type="containsText" dxfId="24" priority="66" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="79" priority="79" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="132" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="78" priority="145" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="214" priority="57" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="77" priority="70" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="58" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="76" priority="71" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="212" priority="59" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="75" priority="72" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="211" priority="60" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="61" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="62" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="208" priority="63" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="71" priority="76" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="64" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="70" priority="77" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="65" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="69" priority="78" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="containsText" dxfId="205" priority="47" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="68" priority="60" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="48" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="67" priority="61" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="203" priority="49" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="66" priority="62" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="50" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="65" priority="63" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="51" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="64" priority="64" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="200" priority="52" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="63" priority="65" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="53" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="62" priority="66" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="54" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="61" priority="67" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="55" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="60" priority="68" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="56" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="59" priority="69" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F16">
-    <cfRule type="containsText" dxfId="195" priority="46" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="194" priority="45" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="193" priority="35" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="56" priority="48" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="36" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="55" priority="49" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="37" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="54" priority="50" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="38" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="53" priority="51" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="39" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="52" priority="52" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="188" priority="40" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="51" priority="53" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="41" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="50" priority="54" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="42" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="49" priority="55" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="43" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="48" priority="56" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="44" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="47" priority="57" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="183" priority="34" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="182" priority="24" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="45" priority="37" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="25" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="44" priority="38" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="26" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="43" priority="39" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="179" priority="27" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="28" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="29" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="176" priority="30" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="31" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="38" priority="44" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="32" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="37" priority="45" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="33" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="36" priority="46" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="172" priority="23" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="171" priority="14" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="34" priority="27" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="15" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="33" priority="28" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="16" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="32" priority="29" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="17" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="18" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="19" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="20" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="21" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="27" priority="34" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="22" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="26" priority="35" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="162" priority="13" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F26">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="23" priority="15" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="22" priority="16" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="21" priority="17" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="15" priority="23" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="14" priority="24" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E26">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
infowindow mouse hoover multiple marker
</commit_message>
<xml_diff>
--- a/src/main/resources/TODOs.xlsx
+++ b/src/main/resources/TODOs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace\incident-app\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849ECC23-D839-4F2C-9B7B-B3F15B13EA23}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910B8302-C2AA-4FD5-898C-008CFD0DF363}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9972" windowHeight="8244" activeTab="2" xr2:uid="{AA738D5C-D5BE-4907-AFCA-ACBAF9B3F897}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -195,13 +195,55 @@
   </si>
   <si>
     <t>load only incidents on a specified radius</t>
+  </si>
+  <si>
+    <t>Final Report Project</t>
+  </si>
+  <si>
+    <t>Report Layout, index, SRS- Software Req Specification</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Infowindow</t>
+  </si>
+  <si>
+    <t>Layout image 1st</t>
+  </si>
+  <si>
+    <t>Increase size to fit the dropdowns</t>
+  </si>
+  <si>
+    <t>Test with a video upload</t>
+  </si>
+  <si>
+    <t>Hover through a multi incident icon shows the quantity of incidents by type</t>
+  </si>
+  <si>
+    <t>View Trends</t>
+  </si>
+  <si>
+    <t>Phone Gap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study </t>
+  </si>
+  <si>
+    <t>create a chart with incidents of the past 12 months - js library</t>
+  </si>
+  <si>
+    <t>Thumbnails square format and the same dimensions - set css</t>
+  </si>
+  <si>
+    <t>Relocate the user and populate incidents around him(if the user is in the same position do not do that)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,8 +265,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,14 +298,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -279,11 +322,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,22 +369,924 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="153">
+  <dxfs count="251">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2334,8 +3290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466B8D82-E7DF-4CF4-AFC0-ECEA7696B0DD}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2450,7 +3406,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>17</v>
@@ -2470,7 +3426,7 @@
         <v>18</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>17</v>
@@ -2488,30 +3444,30 @@
         <v>19</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="9" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="3"/>
+      <c r="D9" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -2686,7 +3642,7 @@
         <v>48</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>17</v>
@@ -2722,7 +3678,7 @@
         <v>42</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>17</v>
@@ -2740,7 +3696,7 @@
         <v>43</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>17</v>
@@ -2758,30 +3714,30 @@
         <v>44</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>17</v>
       </c>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21">
+    <row r="24" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
         <v>23</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="22"/>
+      <c r="D24" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="17"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -2819,23 +3775,23 @@
       </c>
       <c r="F26" s="15"/>
     </row>
-    <row r="27" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="25">
+    <row r="27" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21">
         <v>26</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="22" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="26"/>
+      <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
@@ -2848,7 +3804,7 @@
         <v>51</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>17</v>
@@ -2856,75 +3812,163 @@
       <c r="F28" s="17"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>9</v>
+      </c>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>9</v>
+      </c>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -3274,516 +4318,866 @@
   </sheetData>
   <autoFilter ref="A1:F15" xr:uid="{8ACA0151-78CB-428A-BBDA-F3EEE46416DA}"/>
   <conditionalFormatting sqref="A2:F12">
-    <cfRule type="containsText" dxfId="152" priority="148" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="250" priority="246" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="149" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="249" priority="247" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="150" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="248" priority="248" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="151" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="247" priority="249" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="152" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="246" priority="250" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="153" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="245" priority="251" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="154" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="244" priority="252" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="155" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="243" priority="253" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="156" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="242" priority="254" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="143" priority="137" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="241" priority="235" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="138" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="240" priority="236" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="139" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="239" priority="237" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="140" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="238" priority="238" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="141" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="237" priority="239" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="142" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="236" priority="240" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="143" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="235" priority="241" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="144" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="234" priority="242" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="145" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="233" priority="243" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="146" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="232" priority="244" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="133" priority="127" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="231" priority="225" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="128" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="230" priority="226" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="129" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="229" priority="227" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="130" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="228" priority="228" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="131" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="227" priority="229" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="132" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="226" priority="230" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="133" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="225" priority="231" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="134" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="224" priority="232" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="135" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="223" priority="233" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="136" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="222" priority="234" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="123" priority="117" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="221" priority="215" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="118" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="220" priority="216" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="119" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="219" priority="217" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="120" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="218" priority="218" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="121" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="217" priority="219" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="122" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="216" priority="220" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="123" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="215" priority="221" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="124" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="214" priority="222" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="125" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="213" priority="223" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="126" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="212" priority="224" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="113" priority="82" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="211" priority="180" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="107" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="210" priority="205" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="108" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="209" priority="206" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="109" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="208" priority="207" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="207" priority="208" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="206" priority="209" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="112" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="205" priority="210" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="113" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="204" priority="211" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="114" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="203" priority="212" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="115" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="202" priority="213" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="116" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="201" priority="214" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="containsText" dxfId="102" priority="86" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="200" priority="184" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="97" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="199" priority="195" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="98" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="198" priority="196" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="99" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="197" priority="197" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="100" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="196" priority="198" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="195" priority="199" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="102" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="194" priority="200" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="103" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="193" priority="201" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="104" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="192" priority="202" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="105" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="191" priority="203" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="106" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="190" priority="204" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="containsText" dxfId="91" priority="87" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="189" priority="185" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="88" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="188" priority="186" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="89" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="187" priority="187" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="90" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="186" priority="188" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="91" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="185" priority="189" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="92" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="184" priority="190" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="93" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="183" priority="191" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="94" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="182" priority="192" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="95" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="181" priority="193" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="96" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="180" priority="194" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F80">
-    <cfRule type="containsText" dxfId="81" priority="81" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="179" priority="179" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="147" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="178" priority="245" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="79" priority="72" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="177" priority="170" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="73" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="176" priority="171" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="74" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="175" priority="172" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="75" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="174" priority="173" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="173" priority="174" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="77" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="172" priority="175" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="78" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="171" priority="176" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="79" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="170" priority="177" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="80" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="169" priority="178" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="containsText" dxfId="70" priority="62" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="168" priority="160" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="63" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="167" priority="161" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="64" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="166" priority="162" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="165" priority="163" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="164" priority="164" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="163" priority="165" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="162" priority="166" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="69" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="161" priority="167" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="70" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="160" priority="168" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="71" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="159" priority="169" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F16">
-    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="158" priority="159" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="157" priority="158" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
+    <cfRule type="containsText" dxfId="156" priority="148" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="155" priority="149" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="154" priority="150" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="153" priority="151" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="152" priority="152" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="151" priority="153" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="150" priority="154" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="149" priority="155" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="148" priority="156" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="147" priority="157" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="containsText" dxfId="146" priority="147" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="containsText" dxfId="145" priority="137" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="144" priority="138" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="143" priority="139" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="142" priority="140" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="141" priority="141" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="140" priority="142" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="139" priority="143" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="138" priority="144" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="137" priority="145" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="136" priority="146" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="containsText" dxfId="135" priority="136" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="containsText" dxfId="134" priority="127" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="133" priority="128" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="132" priority="129" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="131" priority="130" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="130" priority="131" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="129" priority="132" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="128" priority="133" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="127" priority="134" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="126" priority="135" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="containsText" dxfId="125" priority="126" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:F26">
+    <cfRule type="containsText" dxfId="124" priority="125" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E26">
+    <cfRule type="containsText" dxfId="123" priority="115" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="122" priority="116" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="121" priority="117" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="118" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="119" priority="119" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="118" priority="120" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="121" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="116" priority="122" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="123" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="124" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E26">
+    <cfRule type="containsText" dxfId="113" priority="114" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="111" priority="112" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="110" priority="102" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="103" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="104" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="107" priority="105" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="106" priority="106" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="107" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="104" priority="108" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="109" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="110" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="101" priority="111" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="containsText" dxfId="99" priority="100" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D29">
+    <cfRule type="containsText" dxfId="98" priority="99" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="containsText" dxfId="97" priority="90" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="96" priority="91" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="95" priority="92" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="93" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="93" priority="94" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="95" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="91" priority="96" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="97" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="98" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="containsText" dxfId="87" priority="88" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="containsText" dxfId="86" priority="87" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:E33">
+    <cfRule type="containsText" dxfId="84" priority="85" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="containsText" dxfId="83" priority="75" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="76" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="81" priority="77" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="78" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="79" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="80" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="81" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="82" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="75" priority="83" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="84" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31:E31">
+    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="containsText" dxfId="71" priority="63" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="64" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="65" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="66" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="67" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="68" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="69" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="70" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="71" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="72" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:E34">
+    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
     <cfRule type="containsText" dxfId="58" priority="50" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="57" priority="51" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="56" priority="52" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="53" priority="55" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",D17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("LOW",E34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="51" priority="57" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HIGH",E34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="50" priority="58" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="49" priority="59" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
     <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="47" priority="39" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="40" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="41" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="42" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="43" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="44" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="45" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="46" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="47" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="48" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="36" priority="29" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="30" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="32" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="34" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="37" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F26">
-    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="25" priority="17" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="18" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D28)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:E35">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="containsText" dxfId="45" priority="37" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="38" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="39" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="44" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="45" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="46" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:E36">
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="containsText" dxfId="32" priority="24" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="31" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="32" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="33" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="21" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="22" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:E37">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
todo updated, infowindow close adjusted and multi incident marker redefined
</commit_message>
<xml_diff>
--- a/src/main/resources/TODOs.xlsx
+++ b/src/main/resources/TODOs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace\incident-app\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910B8302-C2AA-4FD5-898C-008CFD0DF363}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8FF846-B3C3-41D9-AE0D-E16491A234D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9972" windowHeight="8244" activeTab="2" xr2:uid="{AA738D5C-D5BE-4907-AFCA-ACBAF9B3F897}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -215,9 +215,6 @@
     <t>Increase size to fit the dropdowns</t>
   </si>
   <si>
-    <t>Test with a video upload</t>
-  </si>
-  <si>
     <t>Hover through a multi incident icon shows the quantity of incidents by type</t>
   </si>
   <si>
@@ -237,6 +234,21 @@
   </si>
   <si>
     <t>Relocate the user and populate incidents around him(if the user is in the same position do not do that)</t>
+  </si>
+  <si>
+    <t>change multi marker icon</t>
+  </si>
+  <si>
+    <t>when opening infowindow close others</t>
+  </si>
+  <si>
+    <t>Dialog box</t>
+  </si>
+  <si>
+    <t>Resize to fit dropdowns for incident types</t>
+  </si>
+  <si>
+    <t>Test with a video upload - DOES NOT WORK</t>
   </si>
 </sst>
 </file>
@@ -273,7 +285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +307,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,11 +394,148 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="251">
+  <dxfs count="265">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3290,8 +3445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466B8D82-E7DF-4CF4-AFC0-ECEA7696B0DD}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3819,7 +3974,7 @@
         <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>8</v>
@@ -3845,41 +4000,41 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+    <row r="31" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+      <c r="E31" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="27"/>
+    </row>
+    <row r="32" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="16">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>64</v>
+      <c r="C32" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="3"/>
+      <c r="E32" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="17"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
@@ -3899,69 +4054,69 @@
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+    <row r="34" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>58</v>
+      <c r="C34" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+      <c r="E34" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="17"/>
+    </row>
+    <row r="35" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="16">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>59</v>
+      <c r="C35" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="17"/>
+    </row>
+    <row r="36" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="26">
+        <v>35</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="3"/>
+      <c r="F36" s="27"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>14</v>
@@ -3971,28 +4126,58 @@
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+    <row r="38" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="16">
+        <v>37</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="17"/>
+    </row>
+    <row r="39" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
+        <v>38</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -4318,866 +4503,918 @@
   </sheetData>
   <autoFilter ref="A1:F15" xr:uid="{8ACA0151-78CB-428A-BBDA-F3EEE46416DA}"/>
   <conditionalFormatting sqref="A2:F12">
-    <cfRule type="containsText" dxfId="250" priority="246" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="264" priority="260" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="247" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="263" priority="261" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="248" priority="248" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="262" priority="262" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="247" priority="249" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="261" priority="263" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="250" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="260" priority="264" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="251" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="259" priority="265" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="244" priority="252" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="258" priority="266" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="243" priority="253" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="257" priority="267" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="242" priority="254" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="256" priority="268" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="241" priority="235" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="255" priority="249" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="240" priority="236" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="254" priority="250" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="239" priority="237" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="253" priority="251" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="238" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="252" priority="252" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="239" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="251" priority="253" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="236" priority="240" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="250" priority="254" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="235" priority="241" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="249" priority="255" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="242" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="248" priority="256" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="243" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="247" priority="257" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="232" priority="244" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="246" priority="258" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="231" priority="225" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="245" priority="239" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="226" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="244" priority="240" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="227" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="243" priority="241" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="228" priority="228" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="242" priority="242" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="227" priority="229" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="241" priority="243" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="230" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="240" priority="244" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="231" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="239" priority="245" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="224" priority="232" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="238" priority="246" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="223" priority="233" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="237" priority="247" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="234" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="236" priority="248" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="221" priority="215" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="235" priority="229" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="216" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="234" priority="230" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="219" priority="217" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="233" priority="231" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="218" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="232" priority="232" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="219" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="231" priority="233" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="216" priority="220" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="230" priority="234" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="215" priority="221" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="229" priority="235" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="222" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="228" priority="236" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="223" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="227" priority="237" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="212" priority="224" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="226" priority="238" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="211" priority="180" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="225" priority="194" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="205" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="224" priority="219" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="206" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="223" priority="220" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="208" priority="207" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="222" priority="221" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="208" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="221" priority="222" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="209" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="220" priority="223" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="210" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="219" priority="224" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="211" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="218" priority="225" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="203" priority="212" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="217" priority="226" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="213" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="216" priority="227" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="214" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="215" priority="228" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="containsText" dxfId="200" priority="184" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="214" priority="198" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="195" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="213" priority="209" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="196" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="212" priority="210" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="197" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="211" priority="211" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="198" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="210" priority="212" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="199" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="209" priority="213" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="200" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="208" priority="214" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="201" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="207" priority="215" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="202" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="206" priority="216" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="203" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="205" priority="217" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="204" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="204" priority="218" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="containsText" dxfId="189" priority="185" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="203" priority="199" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="188" priority="186" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="202" priority="200" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="187" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="201" priority="201" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="188" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="200" priority="202" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="189" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="199" priority="203" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="190" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="198" priority="204" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="191" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="197" priority="205" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="192" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="196" priority="206" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="193" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="195" priority="207" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="194" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="194" priority="208" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F80">
-    <cfRule type="containsText" dxfId="179" priority="179" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="193" priority="193" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="245" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="192" priority="259" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="177" priority="170" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="191" priority="184" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="176" priority="171" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="190" priority="185" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="172" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="189" priority="186" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="173" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="188" priority="187" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="174" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="187" priority="188" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="175" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="186" priority="189" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="176" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="185" priority="190" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="177" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="184" priority="191" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="178" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="183" priority="192" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="containsText" dxfId="168" priority="160" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="182" priority="174" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="161" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="181" priority="175" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="162" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="180" priority="176" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="163" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="179" priority="177" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="164" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="178" priority="178" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="165" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="177" priority="179" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="166" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="176" priority="180" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="167" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="175" priority="181" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="168" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="174" priority="182" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="169" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="173" priority="183" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F16">
-    <cfRule type="containsText" dxfId="158" priority="159" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="172" priority="173" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="157" priority="158" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="171" priority="172" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="156" priority="148" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="170" priority="162" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="155" priority="149" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="169" priority="163" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="150" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="168" priority="164" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="151" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="167" priority="165" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="152" priority="152" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="166" priority="166" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="153" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="165" priority="167" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="154" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="164" priority="168" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="155" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="163" priority="169" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="156" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="162" priority="170" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="157" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="161" priority="171" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="146" priority="147" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="160" priority="161" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="145" priority="137" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="159" priority="151" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="138" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="158" priority="152" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="139" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="157" priority="153" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="140" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="156" priority="154" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="141" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="155" priority="155" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="142" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="154" priority="156" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="143" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="153" priority="157" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="144" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="152" priority="158" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="145" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="151" priority="159" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="146" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="150" priority="160" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="135" priority="136" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="149" priority="150" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="134" priority="127" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="148" priority="141" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="128" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="147" priority="142" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="129" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="146" priority="143" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="130" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="145" priority="144" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="131" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="144" priority="145" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="132" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="143" priority="146" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="133" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="142" priority="147" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="134" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="141" priority="148" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="135" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="140" priority="149" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="125" priority="126" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="139" priority="140" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F26">
-    <cfRule type="containsText" dxfId="124" priority="125" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="138" priority="139" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="123" priority="115" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="137" priority="129" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="116" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="136" priority="130" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="117" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="135" priority="131" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="118" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="134" priority="132" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="119" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="133" priority="133" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="120" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="132" priority="134" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="121" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="131" priority="135" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="122" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="130" priority="136" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="123" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="129" priority="137" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="124" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="128" priority="138" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="113" priority="114" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="127" priority="128" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
+    <cfRule type="containsText" dxfId="126" priority="127" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="125" priority="126" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="124" priority="116" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="123" priority="117" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="122" priority="118" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="121" priority="119" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="120" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="119" priority="121" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="118" priority="122" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="123" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="116" priority="124" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="125" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="114" priority="115" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="containsText" dxfId="113" priority="114" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D29">
     <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="111" priority="112" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="110" priority="102" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="103" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="104" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="105" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="106" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="107" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="108" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="109" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="110" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="111" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="containsText" dxfId="111" priority="104" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="110" priority="105" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="106" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="107" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="107" priority="108" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="106" priority="109" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="110" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="104" priority="111" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="112" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="containsText" dxfId="102" priority="103" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="containsText" dxfId="101" priority="102" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
     <cfRule type="containsText" dxfId="99" priority="100" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D29">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:E33">
     <cfRule type="containsText" dxfId="98" priority="99" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="97" priority="90" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="91" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="92" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="93" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="94" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="95" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="96" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="97" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="98" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="87" priority="88" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="containsText" dxfId="97" priority="89" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="96" priority="90" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="95" priority="91" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="92" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="93" priority="93" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="94" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="91" priority="95" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="96" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="97" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="98" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="containsText" dxfId="87" priority="88" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31:E31">
     <cfRule type="containsText" dxfId="86" priority="87" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33:E33">
-    <cfRule type="containsText" dxfId="84" priority="85" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="containsText" dxfId="83" priority="75" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="76" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="77" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="78" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="79" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="80" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="81" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="82" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="83" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="84" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31:E31">
-    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" dxfId="71" priority="63" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="85" priority="77" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="64" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="84" priority="78" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="65" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="83" priority="79" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="66" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="82" priority="80" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="67" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="81" priority="81" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="68" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="80" priority="82" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="69" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="70" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="78" priority="84" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="71" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="77" priority="85" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="72" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="76" priority="86" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
+    <cfRule type="containsText" dxfId="74" priority="75" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:E34">
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="containsText" dxfId="72" priority="64" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="71" priority="65" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="66" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="67" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="68" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="69" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="70" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="71" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="72" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="73" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:E35">
     <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34:E34">
-    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="58" priority="50" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="51" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="52" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="55" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="57" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="58" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="59" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="containsText" dxfId="59" priority="51" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="52" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="53" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="54" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="55" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="56" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="57" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="58" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="59" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="60" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:E36">
     <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:E35">
-    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="45" priority="37" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="38" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="39" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="44" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="45" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="46" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:E36">
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="32" priority="24" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="46" priority="38" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="45" priority="39" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="44" priority="40" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="31" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="32" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="38" priority="46" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="33" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="37" priority="47" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="35" priority="28" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="34" priority="29" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="33" priority="30" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="29" priority="34" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="21" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="22" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="27" priority="36" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:E37">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="24" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
     <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
     <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("LOW",E40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update todos, chart layout improvement and style button single incident infowindow
</commit_message>
<xml_diff>
--- a/src/main/resources/TODOs.xlsx
+++ b/src/main/resources/TODOs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace\incident-app\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFBD9408-5C02-4AEA-AAE8-169411A08CCB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E62219-B296-44BC-99FF-C222C3BBB9B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="17748" windowHeight="11640" activeTab="2" xr2:uid="{AA738D5C-D5BE-4907-AFCA-ACBAF9B3F897}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AA738D5C-D5BE-4907-AFCA-ACBAF9B3F897}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,6 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="90">
   <si>
     <t>ID</t>
   </si>
@@ -262,13 +261,61 @@
   </si>
   <si>
     <t>Set up layout html, css</t>
+  </si>
+  <si>
+    <t>One icon for all incidents</t>
+  </si>
+  <si>
+    <t>Combobox dropdown list contatining country, state and city</t>
+  </si>
+  <si>
+    <t>Infowindow: set up message font</t>
+  </si>
+  <si>
+    <t>Infowindow one incident: set up button</t>
+  </si>
+  <si>
+    <t>Infowindow on incident: set up color background</t>
+  </si>
+  <si>
+    <t>Infowindow Multiincident: set up background color</t>
+  </si>
+  <si>
+    <t>Infowindow Multiincident: take off underlined</t>
+  </si>
+  <si>
+    <t>Infowindow bug: hidden infowindow when use dropdown</t>
+  </si>
+  <si>
+    <t>Dialog box: message multiline</t>
+  </si>
+  <si>
+    <t>Dialog box: improve layout (colors)</t>
+  </si>
+  <si>
+    <t>Dialog box: resize to fit mobile</t>
+  </si>
+  <si>
+    <t>Fix click "Go" on mobile keyboard</t>
+  </si>
+  <si>
+    <t>Fix Address autofilling on user registration</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Put logo app </t>
+  </si>
+  <si>
+    <t>Registration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +344,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,6 +386,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -401,22 +461,847 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="293">
+  <dxfs count="380">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3714,10 +4599,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466B8D82-E7DF-4CF4-AFC0-ECEA7696B0DD}">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4165,23 +5050,23 @@
       </c>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20">
+    <row r="25" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="17">
         <v>24</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="21"/>
+      <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -4250,7 +5135,7 @@
       <c r="D29" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="5"/>
@@ -4271,23 +5156,23 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16">
+    <row r="31" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="17"/>
+      <c r="E31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
@@ -4302,28 +5187,28 @@
       <c r="D32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+    <row r="33" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="3"/>
+      <c r="E33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
@@ -4361,23 +5246,23 @@
       </c>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16">
+    <row r="36" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="17"/>
+      <c r="D36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
@@ -4392,7 +5277,7 @@
       <c r="D37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F37" s="5"/>
@@ -4408,7 +5293,7 @@
         <v>65</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>17</v>
@@ -4469,144 +5354,292 @@
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+    <row r="42" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="20">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" s="21"/>
+    </row>
+    <row r="43" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="24">
+        <v>42</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" s="25"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+    <row r="46" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -4777,1041 +5810,1358 @@
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:F15" xr:uid="{8ACA0151-78CB-428A-BBDA-F3EEE46416DA}"/>
   <conditionalFormatting sqref="A2:F12">
-    <cfRule type="containsText" dxfId="292" priority="288" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="379" priority="410" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="291" priority="289" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="378" priority="411" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="290" priority="290" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="377" priority="412" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="289" priority="291" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="376" priority="413" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="288" priority="292" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="375" priority="414" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="287" priority="293" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="374" priority="415" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="286" priority="294" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="373" priority="416" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="285" priority="295" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="372" priority="417" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="284" priority="296" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="371" priority="418" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="containsText" dxfId="283" priority="277" operator="containsText" text="DONE">
+  <conditionalFormatting sqref="D13 E45:E57">
+    <cfRule type="containsText" dxfId="370" priority="399" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="278" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="369" priority="400" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="281" priority="279" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="368" priority="401" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="280" priority="280" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="367" priority="402" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="279" priority="281" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="366" priority="403" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="278" priority="282" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="365" priority="404" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="283" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="364" priority="405" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="276" priority="284" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="363" priority="406" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="275" priority="285" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="362" priority="407" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="274" priority="286" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="361" priority="408" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="273" priority="267" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="360" priority="389" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="272" priority="268" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="359" priority="390" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="271" priority="269" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="358" priority="391" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="270" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="357" priority="392" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="271" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="356" priority="393" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="268" priority="272" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="355" priority="394" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="267" priority="273" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="354" priority="395" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="266" priority="274" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="353" priority="396" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="275" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="352" priority="397" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="264" priority="276" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="351" priority="398" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="263" priority="257" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="350" priority="379" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="258" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="349" priority="380" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="259" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="348" priority="381" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="260" priority="260" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="347" priority="382" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="259" priority="261" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="346" priority="383" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="262" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="345" priority="384" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="263" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="344" priority="385" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="256" priority="264" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="343" priority="386" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="255" priority="265" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="342" priority="387" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="254" priority="266" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="341" priority="388" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="253" priority="222" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="340" priority="344" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="252" priority="247" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="339" priority="369" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="251" priority="248" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="338" priority="370" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="249" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="337" priority="371" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="250" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="336" priority="372" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="248" priority="251" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="335" priority="373" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="247" priority="252" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="334" priority="374" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="253" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="333" priority="375" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="254" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="332" priority="376" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="244" priority="255" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="331" priority="377" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="243" priority="256" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="330" priority="378" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="containsText" dxfId="242" priority="226" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="329" priority="348" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="237" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="328" priority="359" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="240" priority="238" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="327" priority="360" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="239" priority="239" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="326" priority="361" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="240" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="325" priority="362" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="241" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="324" priority="363" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="236" priority="242" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="323" priority="364" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="235" priority="243" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="322" priority="365" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="244" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="321" priority="366" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="245" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="320" priority="367" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="232" priority="246" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="319" priority="368" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="containsText" dxfId="231" priority="227" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="318" priority="349" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="228" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="317" priority="350" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="229" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="316" priority="351" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="228" priority="230" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="315" priority="352" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="227" priority="231" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="314" priority="353" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="232" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="313" priority="354" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="233" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="312" priority="355" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="224" priority="234" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="311" priority="356" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="223" priority="235" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="310" priority="357" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="236" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="309" priority="358" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F80">
-    <cfRule type="containsText" dxfId="221" priority="221" operator="containsText" text="IN PROGRESS">
+  <conditionalFormatting sqref="A2:F78">
+    <cfRule type="containsText" dxfId="308" priority="343" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="287" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="307" priority="409" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="219" priority="212" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="306" priority="334" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="213" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="305" priority="335" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="214" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="304" priority="336" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="216" priority="215" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="303" priority="337" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="215" priority="216" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="302" priority="338" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="217" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="301" priority="339" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="218" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="300" priority="340" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="212" priority="219" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="299" priority="341" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="211" priority="220" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="298" priority="342" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="containsText" dxfId="210" priority="202" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="297" priority="324" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="203" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="296" priority="325" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="208" priority="204" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="295" priority="326" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="205" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="294" priority="327" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="206" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="293" priority="328" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="207" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="292" priority="329" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="208" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="291" priority="330" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="203" priority="209" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="290" priority="331" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="210" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="289" priority="332" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="211" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="288" priority="333" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F16">
-    <cfRule type="containsText" dxfId="200" priority="201" operator="containsText" text="DONE">
+  <conditionalFormatting sqref="A2:F16 E45:E57">
+    <cfRule type="containsText" dxfId="287" priority="323" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="199" priority="200" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="286" priority="322" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="198" priority="190" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="285" priority="312" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="191" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="284" priority="313" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="192" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="283" priority="314" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="193" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="282" priority="315" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="194" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="281" priority="316" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="195" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="280" priority="317" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="196" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="279" priority="318" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="197" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="278" priority="319" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="198" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="277" priority="320" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="199" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="276" priority="321" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="188" priority="189" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="275" priority="311" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="187" priority="179" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="274" priority="301" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="180" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="273" priority="302" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="181" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="272" priority="303" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="182" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="271" priority="304" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="183" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="270" priority="305" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="184" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="269" priority="306" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="185" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="268" priority="307" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="186" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="267" priority="308" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="179" priority="187" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="266" priority="309" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="188" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="265" priority="310" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="177" priority="178" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="264" priority="300" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="176" priority="169" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="263" priority="291" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="170" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="262" priority="292" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="171" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="261" priority="293" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="172" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="260" priority="294" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="173" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="259" priority="295" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="174" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="258" priority="296" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="175" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="257" priority="297" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="176" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="256" priority="298" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="177" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="255" priority="299" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="167" priority="168" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="254" priority="290" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F26">
-    <cfRule type="containsText" dxfId="166" priority="167" operator="containsText" text="HIGH">
+  <conditionalFormatting sqref="A2:F26 E45:E57">
+    <cfRule type="containsText" dxfId="253" priority="289" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="165" priority="157" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="252" priority="279" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="158" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="251" priority="280" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="159" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="250" priority="281" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="160" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="249" priority="282" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="161" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="248" priority="283" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="162" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="247" priority="284" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="163" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="246" priority="285" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="164" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="245" priority="286" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="165" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="244" priority="287" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="166" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="243" priority="288" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="155" priority="156" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="242" priority="278" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="containsText" dxfId="154" priority="155" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="241" priority="277" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="153" priority="154" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="240" priority="276" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="152" priority="144" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="239" priority="266" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="145" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="238" priority="267" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="146" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="237" priority="268" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="147" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="236" priority="269" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="148" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="235" priority="270" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="149" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="234" priority="271" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="150" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="233" priority="272" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="151" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="232" priority="273" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="152" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="231" priority="274" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="153" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="230" priority="275" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="142" priority="143" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="229" priority="265" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="containsText" dxfId="141" priority="142" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="228" priority="264" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:D29">
-    <cfRule type="containsText" dxfId="140" priority="141" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="227" priority="263" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="139" priority="132" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="226" priority="254" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="133" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="225" priority="255" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="134" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="224" priority="256" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="135" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="223" priority="257" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="136" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="222" priority="258" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="137" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="221" priority="259" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="138" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="220" priority="260" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="139" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="219" priority="261" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="140" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="218" priority="262" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="130" priority="131" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="217" priority="253" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="129" priority="130" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="216" priority="252" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="containsText" dxfId="128" priority="129" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="215" priority="251" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="containsText" dxfId="127" priority="128" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="214" priority="250" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:E33">
-    <cfRule type="containsText" dxfId="126" priority="127" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="213" priority="249" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="containsText" dxfId="125" priority="117" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="212" priority="239" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="118" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="211" priority="240" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="119" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="210" priority="241" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="120" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="209" priority="242" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="121" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="208" priority="243" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="122" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="207" priority="244" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="123" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="206" priority="245" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="124" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="205" priority="246" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="125" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="204" priority="247" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="126" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="203" priority="248" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="containsText" dxfId="115" priority="116" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="202" priority="238" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:E31">
-    <cfRule type="containsText" dxfId="114" priority="115" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="201" priority="237" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" dxfId="113" priority="105" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="200" priority="227" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="106" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="199" priority="228" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="107" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="198" priority="229" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="108" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="197" priority="230" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="109" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="196" priority="231" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="110" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="195" priority="232" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="111" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="194" priority="233" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="112" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="193" priority="234" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="113" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="192" priority="235" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="114" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="191" priority="236" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" dxfId="103" priority="104" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="190" priority="226" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="102" priority="103" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="189" priority="225" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:E34">
-    <cfRule type="containsText" dxfId="101" priority="102" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="188" priority="224" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="100" priority="92" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="187" priority="214" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="93" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="186" priority="215" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="94" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="185" priority="216" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="95" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="184" priority="217" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="96" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="183" priority="218" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="97" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="182" priority="219" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="181" priority="220" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="99" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="180" priority="221" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="100" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="179" priority="222" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="101" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="178" priority="223" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="90" priority="91" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="177" priority="213" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="containsText" dxfId="89" priority="90" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="176" priority="212" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:E35">
-    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="175" priority="211" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="87" priority="79" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="174" priority="201" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="80" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="173" priority="202" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="81" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="172" priority="203" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="82" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="171" priority="204" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="83" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="170" priority="205" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="84" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="169" priority="206" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="85" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="168" priority="207" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="86" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="167" priority="208" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="87" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="166" priority="209" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="88" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="165" priority="210" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="164" priority="200" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="163" priority="199" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36:E36">
-    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="162" priority="198" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="74" priority="66" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="161" priority="188" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="67" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="160" priority="189" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="68" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="159" priority="190" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="69" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="158" priority="191" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="70" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="157" priority="192" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="71" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="156" priority="193" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="72" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="155" priority="194" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="73" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="154" priority="195" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="74" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="153" priority="196" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="75" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="152" priority="197" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="151" priority="187" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="63" priority="56" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="150" priority="178" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="57" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="149" priority="179" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="58" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="148" priority="180" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="59" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="147" priority="181" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="146" priority="182" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="61" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="145" priority="183" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="62" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="144" priority="184" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="63" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="143" priority="185" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="64" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="142" priority="186" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="141" priority="177" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:E37">
-    <cfRule type="containsText" dxfId="53" priority="54" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="140" priority="176" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" dxfId="52" priority="44" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="139" priority="166" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="45" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="138" priority="167" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="137" priority="168" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="136" priority="169" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="135" priority="170" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="49" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="134" priority="171" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="133" priority="172" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="51" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="132" priority="173" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="52" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="131" priority="174" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="53" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="130" priority="175" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="129" priority="165" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="128" priority="164" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="127" priority="163" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="126" priority="162" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="38" priority="30" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="125" priority="152" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="31" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="124" priority="153" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="32" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="123" priority="154" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="122" priority="155" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="121" priority="156" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="120" priority="157" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="119" priority="158" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="118" priority="159" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="38" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="117" priority="160" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="39" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="116" priority="161" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="115" priority="151" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="114" priority="150" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="113" priority="149" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="112" priority="148" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="111" priority="138" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="110" priority="139" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="109" priority="140" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="108" priority="141" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="107" priority="142" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="106" priority="143" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="105" priority="144" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="104" priority="145" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="24" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="103" priority="146" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="102" priority="147" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="101" priority="137" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="100" priority="136" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
+    <cfRule type="containsText" dxfId="99" priority="135" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="98" priority="134" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="97" priority="124" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="96" priority="125" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="95" priority="126" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="94" priority="127" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="93" priority="128" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="129" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="91" priority="130" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="131" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="132" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="133" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="87" priority="123" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:D44">
+    <cfRule type="containsText" dxfId="86" priority="122" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:D44">
+    <cfRule type="containsText" dxfId="85" priority="121" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="84" priority="120" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="83" priority="110" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="111" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="81" priority="112" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="113" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="114" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="115" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="116" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="117" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="75" priority="118" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="119" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="73" priority="109" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" dxfId="72" priority="108" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" dxfId="71" priority="98" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="99" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="100" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="101" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="102" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="103" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="104" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="105" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="106" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="107" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" dxfId="61" priority="97" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="containsText" dxfId="60" priority="84" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="containsText" dxfId="59" priority="83" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="containsText" dxfId="58" priority="82" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="containsText" dxfId="57" priority="81" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="containsText" dxfId="56" priority="80" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="containsText" dxfId="55" priority="79" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="containsText" dxfId="54" priority="78" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="containsText" dxfId="53" priority="77" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="containsText" dxfId="52" priority="76" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="containsText" dxfId="51" priority="75" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="containsText" dxfId="50" priority="74" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="containsText" dxfId="49" priority="73" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="48" priority="64" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="65" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="66" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="67" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="68" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="69" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="70" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="71" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="72" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="39" priority="63" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="38" priority="62" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="containsText" dxfId="37" priority="50" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="containsText" dxfId="36" priority="49" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="containsText" dxfId="34" priority="47" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="containsText" dxfId="33" priority="38" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="40" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="43" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="44" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="45" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="46" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="containsText" dxfId="24" priority="37" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="containsText" dxfId="23" priority="36" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="22" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="23" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
     <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
     <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
     <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E46)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E46)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("LOW",E46)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HIGH",E46)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change styles elements in infowindow
</commit_message>
<xml_diff>
--- a/src/main/resources/TODOs.xlsx
+++ b/src/main/resources/TODOs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace\incident-app\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E62219-B296-44BC-99FF-C222C3BBB9B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EA7115-F7E3-43CB-8207-4CC3E413FAAC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AA738D5C-D5BE-4907-AFCA-ACBAF9B3F897}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>Registration</t>
+  </si>
+  <si>
+    <t>Modal image</t>
+  </si>
+  <si>
+    <t>set up "x" close style</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,220 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="380">
+  <dxfs count="403">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -4602,7 +4821,7 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5644,10 +5863,18 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
+      <c r="B58" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -5813,1355 +6040,1436 @@
   </sheetData>
   <autoFilter ref="A1:F15" xr:uid="{8ACA0151-78CB-428A-BBDA-F3EEE46416DA}"/>
   <conditionalFormatting sqref="A2:F12">
-    <cfRule type="containsText" dxfId="379" priority="410" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="402" priority="433" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="378" priority="411" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="401" priority="434" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="377" priority="412" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="400" priority="435" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="376" priority="413" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="399" priority="436" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="375" priority="414" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="398" priority="437" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="374" priority="415" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="397" priority="438" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="373" priority="416" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="396" priority="439" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="372" priority="417" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="395" priority="440" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="371" priority="418" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="394" priority="441" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 E45:E57">
-    <cfRule type="containsText" dxfId="370" priority="399" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="393" priority="422" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="369" priority="400" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="392" priority="423" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="368" priority="401" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="391" priority="424" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="367" priority="402" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="390" priority="425" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="366" priority="403" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="389" priority="426" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="365" priority="404" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="388" priority="427" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="364" priority="405" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="387" priority="428" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="363" priority="406" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="386" priority="429" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="362" priority="407" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="385" priority="430" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="361" priority="408" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="384" priority="431" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="360" priority="389" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="383" priority="412" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="359" priority="390" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="382" priority="413" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="358" priority="391" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="381" priority="414" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="357" priority="392" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="380" priority="415" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="356" priority="393" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="379" priority="416" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="355" priority="394" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="378" priority="417" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="354" priority="395" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="377" priority="418" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="353" priority="396" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="376" priority="419" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="352" priority="397" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="375" priority="420" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="351" priority="398" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="374" priority="421" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="350" priority="379" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="373" priority="402" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="349" priority="380" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="372" priority="403" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="348" priority="381" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="371" priority="404" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="347" priority="382" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="370" priority="405" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="346" priority="383" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="369" priority="406" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="345" priority="384" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="368" priority="407" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="344" priority="385" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="367" priority="408" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="343" priority="386" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="366" priority="409" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="342" priority="387" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="365" priority="410" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="341" priority="388" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="364" priority="411" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="340" priority="344" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="363" priority="367" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="339" priority="369" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="362" priority="392" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="338" priority="370" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="361" priority="393" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="337" priority="371" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="360" priority="394" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="336" priority="372" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="359" priority="395" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="335" priority="373" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="358" priority="396" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="334" priority="374" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="357" priority="397" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="333" priority="375" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="356" priority="398" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="332" priority="376" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="355" priority="399" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="331" priority="377" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="354" priority="400" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="330" priority="378" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="353" priority="401" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="containsText" dxfId="329" priority="348" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="352" priority="371" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="328" priority="359" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="351" priority="382" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="327" priority="360" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="350" priority="383" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="326" priority="361" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="349" priority="384" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="325" priority="362" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="348" priority="385" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="324" priority="363" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="347" priority="386" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="323" priority="364" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="346" priority="387" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="322" priority="365" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="345" priority="388" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="321" priority="366" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="344" priority="389" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="320" priority="367" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="343" priority="390" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="319" priority="368" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="342" priority="391" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="containsText" dxfId="318" priority="349" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="341" priority="372" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="317" priority="350" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="340" priority="373" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="316" priority="351" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="339" priority="374" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="315" priority="352" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="338" priority="375" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="314" priority="353" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="337" priority="376" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="313" priority="354" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="336" priority="377" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="312" priority="355" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="335" priority="378" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="311" priority="356" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="334" priority="379" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="310" priority="357" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="333" priority="380" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="309" priority="358" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="332" priority="381" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F78">
-    <cfRule type="containsText" dxfId="308" priority="343" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="331" priority="366" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="307" priority="409" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="330" priority="432" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="306" priority="334" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="329" priority="357" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="305" priority="335" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="328" priority="358" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="304" priority="336" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="327" priority="359" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="303" priority="337" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="326" priority="360" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="302" priority="338" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="325" priority="361" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="301" priority="339" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="324" priority="362" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="300" priority="340" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="323" priority="363" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="299" priority="341" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="322" priority="364" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="298" priority="342" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="321" priority="365" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
+    <cfRule type="containsText" dxfId="320" priority="347" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="319" priority="348" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="318" priority="349" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="317" priority="350" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="316" priority="351" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="315" priority="352" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="314" priority="353" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="313" priority="354" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="312" priority="355" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="311" priority="356" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:F16 E45:E57">
+    <cfRule type="containsText" dxfId="310" priority="346" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="containsText" dxfId="309" priority="345" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="containsText" dxfId="308" priority="335" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="307" priority="336" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="306" priority="337" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="305" priority="338" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="304" priority="339" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="303" priority="340" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="302" priority="341" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="301" priority="342" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="300" priority="343" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="299" priority="344" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="containsText" dxfId="298" priority="334" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
     <cfRule type="containsText" dxfId="297" priority="324" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="296" priority="325" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="295" priority="326" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="294" priority="327" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="293" priority="328" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="292" priority="329" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("LOW",E17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="291" priority="330" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="290" priority="331" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HIGH",E17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="289" priority="332" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="288" priority="333" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F16 E45:E57">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
     <cfRule type="containsText" dxfId="287" priority="323" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="286" priority="322" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",B17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="285" priority="312" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="284" priority="313" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="283" priority="314" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="315" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="281" priority="316" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="280" priority="317" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="279" priority="318" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="278" priority="319" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="277" priority="320" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="276" priority="321" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="275" priority="311" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="274" priority="301" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="302" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="272" priority="303" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="271" priority="304" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="305" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="306" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="268" priority="307" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="267" priority="308" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="266" priority="309" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="265" priority="310" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="264" priority="300" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="263" priority="291" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="286" priority="314" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="292" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="285" priority="315" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="293" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="284" priority="316" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="260" priority="294" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="283" priority="317" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="259" priority="295" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="282" priority="318" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="296" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="281" priority="319" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="297" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="280" priority="320" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="256" priority="298" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="279" priority="321" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="255" priority="299" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="278" priority="322" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="254" priority="290" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="277" priority="313" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F26 E45:E57">
-    <cfRule type="containsText" dxfId="253" priority="289" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="276" priority="312" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="252" priority="279" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="275" priority="302" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="251" priority="280" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="274" priority="303" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="281" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="273" priority="304" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="249" priority="282" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="272" priority="305" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="248" priority="283" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="271" priority="306" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="247" priority="284" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="270" priority="307" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="285" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="269" priority="308" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="286" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="268" priority="309" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="244" priority="287" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="267" priority="310" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="243" priority="288" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="266" priority="311" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="242" priority="278" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="265" priority="301" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="containsText" dxfId="241" priority="277" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="264" priority="300" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="240" priority="276" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="263" priority="299" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="239" priority="266" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="262" priority="289" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="267" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="261" priority="290" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="237" priority="268" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="260" priority="291" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="236" priority="269" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="259" priority="292" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="235" priority="270" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="258" priority="293" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="271" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="257" priority="294" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="272" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="256" priority="295" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="232" priority="273" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="255" priority="296" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="231" priority="274" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="254" priority="297" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="275" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="253" priority="298" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="229" priority="265" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="252" priority="288" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="containsText" dxfId="228" priority="264" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="251" priority="287" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:D29">
-    <cfRule type="containsText" dxfId="227" priority="263" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="250" priority="286" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="226" priority="254" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="249" priority="277" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="225" priority="255" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="248" priority="278" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="224" priority="256" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="247" priority="279" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="223" priority="257" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="246" priority="280" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="258" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="245" priority="281" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="259" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="244" priority="282" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="260" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="243" priority="283" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="219" priority="261" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="242" priority="284" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="262" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="241" priority="285" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="217" priority="253" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="240" priority="276" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="216" priority="252" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="239" priority="275" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="containsText" dxfId="215" priority="251" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="238" priority="274" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="containsText" dxfId="214" priority="250" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="237" priority="273" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:E33">
-    <cfRule type="containsText" dxfId="213" priority="249" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="236" priority="272" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="containsText" dxfId="212" priority="239" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="235" priority="262" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="211" priority="240" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="234" priority="263" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="241" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="233" priority="264" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="242" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="232" priority="265" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="208" priority="243" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="231" priority="266" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="244" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="230" priority="267" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="245" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="229" priority="268" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="246" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="228" priority="269" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="247" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="227" priority="270" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="203" priority="248" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="226" priority="271" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="containsText" dxfId="202" priority="238" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="225" priority="261" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:E31">
-    <cfRule type="containsText" dxfId="201" priority="237" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="224" priority="260" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" dxfId="200" priority="227" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="223" priority="250" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="228" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="222" priority="251" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="229" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="221" priority="252" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="230" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="220" priority="253" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="231" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="219" priority="254" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="232" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="218" priority="255" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="233" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="217" priority="256" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="234" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="216" priority="257" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="235" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="215" priority="258" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="236" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="214" priority="259" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" dxfId="190" priority="226" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="213" priority="249" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="189" priority="225" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="212" priority="248" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:E34">
-    <cfRule type="containsText" dxfId="188" priority="224" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="211" priority="247" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="187" priority="214" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="210" priority="237" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="215" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="209" priority="238" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="216" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="208" priority="239" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="217" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="207" priority="240" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="218" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="206" priority="241" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="219" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="205" priority="242" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="220" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="204" priority="243" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="221" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="203" priority="244" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="179" priority="222" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="202" priority="245" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="223" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="201" priority="246" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="177" priority="213" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="200" priority="236" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="containsText" dxfId="176" priority="212" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="199" priority="235" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:E35">
-    <cfRule type="containsText" dxfId="175" priority="211" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="198" priority="234" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="174" priority="201" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="197" priority="224" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="202" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="196" priority="225" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="203" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="195" priority="226" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="204" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="194" priority="227" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="205" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="193" priority="228" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="206" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="192" priority="229" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="207" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="191" priority="230" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="208" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="190" priority="231" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="209" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="189" priority="232" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="210" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="188" priority="233" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
+    <cfRule type="containsText" dxfId="187" priority="223" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="containsText" dxfId="186" priority="222" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:E36">
+    <cfRule type="containsText" dxfId="185" priority="221" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="containsText" dxfId="184" priority="211" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="183" priority="212" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="182" priority="213" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="181" priority="214" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="180" priority="215" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="179" priority="216" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="178" priority="217" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="177" priority="218" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="176" priority="219" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="175" priority="220" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="containsText" dxfId="174" priority="210" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="containsText" dxfId="173" priority="201" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="172" priority="202" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="171" priority="203" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="170" priority="204" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="169" priority="205" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="168" priority="206" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="167" priority="207" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="166" priority="208" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="165" priority="209" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
     <cfRule type="containsText" dxfId="164" priority="200" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:E37">
+    <cfRule type="containsText" dxfId="163" priority="199" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" dxfId="162" priority="189" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="161" priority="190" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="160" priority="191" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="159" priority="192" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="158" priority="193" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="157" priority="194" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="156" priority="195" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="155" priority="196" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="154" priority="197" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="153" priority="198" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" dxfId="152" priority="188" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="containsText" dxfId="151" priority="187" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="containsText" dxfId="150" priority="186" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsText" dxfId="149" priority="185" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsText" dxfId="148" priority="175" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="147" priority="176" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="146" priority="177" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="145" priority="178" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="144" priority="179" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="143" priority="180" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="142" priority="181" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="141" priority="182" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="140" priority="183" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="139" priority="184" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsText" dxfId="138" priority="174" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="containsText" dxfId="137" priority="173" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="containsText" dxfId="136" priority="172" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="containsText" dxfId="135" priority="171" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="containsText" dxfId="134" priority="161" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="133" priority="162" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="132" priority="163" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="131" priority="164" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="130" priority="165" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="129" priority="166" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="128" priority="167" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="127" priority="168" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="126" priority="169" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="125" priority="170" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="containsText" dxfId="124" priority="160" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="containsText" dxfId="123" priority="159" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="containsText" dxfId="122" priority="158" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="121" priority="157" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="120" priority="147" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="119" priority="148" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="118" priority="149" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="150" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="116" priority="151" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="152" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="153" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="113" priority="154" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="155" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="111" priority="156" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="110" priority="146" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:D44">
+    <cfRule type="containsText" dxfId="109" priority="145" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:D44">
+    <cfRule type="containsText" dxfId="108" priority="144" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="107" priority="143" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="106" priority="133" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="134" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="104" priority="135" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="136" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="137" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="101" priority="138" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="139" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="140" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="98" priority="141" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="142" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="96" priority="132" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" dxfId="95" priority="131" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" dxfId="94" priority="121" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="93" priority="122" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="123" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="91" priority="124" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="125" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="126" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="88" priority="127" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="87" priority="128" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="86" priority="129" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="85" priority="130" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" dxfId="84" priority="120" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="containsText" dxfId="83" priority="107" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="containsText" dxfId="82" priority="106" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="163" priority="199" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="81" priority="105" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:E36">
-    <cfRule type="containsText" dxfId="162" priority="198" operator="containsText" text="HIGH">
+  <conditionalFormatting sqref="D36">
+    <cfRule type="containsText" dxfId="80" priority="104" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="161" priority="188" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="189" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="190" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="191" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="192" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="193" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="155" priority="194" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="195" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="196" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="152" priority="197" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="151" priority="187" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="150" priority="178" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="179" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="180" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="181" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="182" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="183" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="184" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="185" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="186" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="141" priority="177" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37:E37">
-    <cfRule type="containsText" dxfId="140" priority="176" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" dxfId="139" priority="166" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="167" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="168" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="169" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="170" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="171" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="172" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="173" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="174" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="175" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" dxfId="129" priority="165" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="128" priority="164" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="127" priority="163" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="126" priority="162" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="125" priority="152" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="153" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="154" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="155" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="156" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="157" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="158" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="159" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="160" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="161" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="115" priority="151" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="114" priority="150" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="113" priority="149" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="112" priority="148" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="111" priority="138" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="139" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="140" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="141" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="142" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="143" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="144" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="145" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="146" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="147" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="101" priority="137" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="containsText" dxfId="100" priority="136" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="containsText" dxfId="99" priority="135" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="98" priority="134" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="97" priority="124" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="125" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="126" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="127" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="128" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="129" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="130" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="131" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="132" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="133" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="87" priority="123" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43:D44">
-    <cfRule type="containsText" dxfId="86" priority="122" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43:D44">
-    <cfRule type="containsText" dxfId="85" priority="121" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="84" priority="120" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="83" priority="110" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="111" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="112" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="113" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="114" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="115" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="116" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="117" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="118" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="119" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="73" priority="109" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="72" priority="108" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="71" priority="98" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="99" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="100" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="101" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="102" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="103" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="104" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="105" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="106" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="107" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="61" priority="97" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="containsText" dxfId="60" priority="84" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="containsText" dxfId="59" priority="83" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="58" priority="82" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="57" priority="81" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="containsText" dxfId="56" priority="80" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="79" priority="103" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="containsText" dxfId="55" priority="79" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="78" priority="102" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="containsText" dxfId="54" priority="78" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="77" priority="101" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="containsText" dxfId="53" priority="77" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="76" priority="100" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
-    <cfRule type="containsText" dxfId="52" priority="76" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="75" priority="99" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
-    <cfRule type="containsText" dxfId="51" priority="75" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="74" priority="98" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57">
-    <cfRule type="containsText" dxfId="50" priority="74" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="73" priority="97" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57">
-    <cfRule type="containsText" dxfId="49" priority="73" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="72" priority="96" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="48" priority="64" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="71" priority="87" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="65" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="70" priority="88" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="66" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="69" priority="89" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="67" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="68" priority="90" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="68" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="67" priority="91" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="69" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="66" priority="92" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="70" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="65" priority="93" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="71" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="64" priority="94" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="72" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="63" priority="95" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="39" priority="63" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="62" priority="86" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="38" priority="62" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="61" priority="85" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="37" priority="50" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="60" priority="73" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="36" priority="49" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="59" priority="72" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="35" priority="48" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="58" priority="71" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="34" priority="47" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="57" priority="70" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="33" priority="38" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="56" priority="61" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="55" priority="62" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="40" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="54" priority="63" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="41" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="53" priority="64" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="42" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="52" priority="65" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="43" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="51" priority="66" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="44" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="50" priority="67" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="45" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="49" priority="68" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="46" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="48" priority="69" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="24" priority="37" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="47" priority="60" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="23" priority="36" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="46" priority="59" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
+    <cfRule type="containsText" dxfId="45" priority="38" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="39" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="40" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="41" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="43" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="44" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="45" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="46" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46">
+    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
+    <cfRule type="containsText" dxfId="33" priority="25" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="26" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="27" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="28" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="33" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="34" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
     <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",D58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",D58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",D46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("LOW",D58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",D58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HIGH",D58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="15" priority="22" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",D58)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="23" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
     <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
+      <formula>NOT(ISERROR(SEARCH("DONE",D58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
     <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HIGH",D58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
condition login before report an incident
</commit_message>
<xml_diff>
--- a/src/main/resources/TODOs.xlsx
+++ b/src/main/resources/TODOs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace\incident-app\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EA7115-F7E3-43CB-8207-4CC3E413FAAC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F300B5F-495A-4E45-913B-125008EBC1FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AA738D5C-D5BE-4907-AFCA-ACBAF9B3F897}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="17748" windowHeight="11640" activeTab="2" xr2:uid="{AA738D5C-D5BE-4907-AFCA-ACBAF9B3F897}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -315,6 +316,9 @@
   </si>
   <si>
     <t>set up "x" close style</t>
+  </si>
+  <si>
+    <t>Put condition user login to report incident</t>
   </si>
 </sst>
 </file>
@@ -440,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -484,11 +488,142 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="403">
+  <dxfs count="417">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7A1E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8CCF5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4821,7 +4956,7 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5627,23 +5762,23 @@
       </c>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
+    <row r="45" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="3"/>
+      <c r="E45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
@@ -5699,23 +5834,23 @@
       </c>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
+    <row r="49" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="3"/>
+      <c r="E49" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
@@ -5735,23 +5870,23 @@
       </c>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
+    <row r="51" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="3"/>
+      <c r="E51" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
@@ -5862,7 +5997,9 @@
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
       <c r="B58" s="3" t="s">
         <v>90</v>
       </c>
@@ -5878,11 +6015,21 @@
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -6040,1436 +6187,1488 @@
   </sheetData>
   <autoFilter ref="A1:F15" xr:uid="{8ACA0151-78CB-428A-BBDA-F3EEE46416DA}"/>
   <conditionalFormatting sqref="A2:F12">
-    <cfRule type="containsText" dxfId="402" priority="433" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="416" priority="447" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="401" priority="434" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="415" priority="448" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="400" priority="435" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="414" priority="449" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="399" priority="436" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="413" priority="450" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="398" priority="437" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="412" priority="451" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="397" priority="438" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="411" priority="452" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="396" priority="439" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="410" priority="453" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="395" priority="440" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="409" priority="454" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="394" priority="441" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="408" priority="455" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 E45:E57">
-    <cfRule type="containsText" dxfId="393" priority="422" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="407" priority="436" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="392" priority="423" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="406" priority="437" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="391" priority="424" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="405" priority="438" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="390" priority="425" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="404" priority="439" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="389" priority="426" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="403" priority="440" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="388" priority="427" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="402" priority="441" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="387" priority="428" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="401" priority="442" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="386" priority="429" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="400" priority="443" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="385" priority="430" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="399" priority="444" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="384" priority="431" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="398" priority="445" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="containsText" dxfId="383" priority="412" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="397" priority="426" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="382" priority="413" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="396" priority="427" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="381" priority="414" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="395" priority="428" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="380" priority="415" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="394" priority="429" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="379" priority="416" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="393" priority="430" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="378" priority="417" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="392" priority="431" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="377" priority="418" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="391" priority="432" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="376" priority="419" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="390" priority="433" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="375" priority="420" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="389" priority="434" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="374" priority="421" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="388" priority="435" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="containsText" dxfId="373" priority="402" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="387" priority="416" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="372" priority="403" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="386" priority="417" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="371" priority="404" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="385" priority="418" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="370" priority="405" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="384" priority="419" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="369" priority="406" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="383" priority="420" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="368" priority="407" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="382" priority="421" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="367" priority="408" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="381" priority="422" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="366" priority="409" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="380" priority="423" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="365" priority="410" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="379" priority="424" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="364" priority="411" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="378" priority="425" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="containsText" dxfId="363" priority="367" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="377" priority="381" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="362" priority="392" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="376" priority="406" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="361" priority="393" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="375" priority="407" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="360" priority="394" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="374" priority="408" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="359" priority="395" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="373" priority="409" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="358" priority="396" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="372" priority="410" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="357" priority="397" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="371" priority="411" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="356" priority="398" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="370" priority="412" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="355" priority="399" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="369" priority="413" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="354" priority="400" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="368" priority="414" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="353" priority="401" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="367" priority="415" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="containsText" dxfId="352" priority="371" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="366" priority="385" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="351" priority="382" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="365" priority="396" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="350" priority="383" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="364" priority="397" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="349" priority="384" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="363" priority="398" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="348" priority="385" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="362" priority="399" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="347" priority="386" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="361" priority="400" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="346" priority="387" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="360" priority="401" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="345" priority="388" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="359" priority="402" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="344" priority="389" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="358" priority="403" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="343" priority="390" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="357" priority="404" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="342" priority="391" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="356" priority="405" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="containsText" dxfId="341" priority="372" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="355" priority="386" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="340" priority="373" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="354" priority="387" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="339" priority="374" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="353" priority="388" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="338" priority="375" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="352" priority="389" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="337" priority="376" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="351" priority="390" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="336" priority="377" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="350" priority="391" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="335" priority="378" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="349" priority="392" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="334" priority="379" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="348" priority="393" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="333" priority="380" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="347" priority="394" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="332" priority="381" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="346" priority="395" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F78">
-    <cfRule type="containsText" dxfId="331" priority="366" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="345" priority="380" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="330" priority="432" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="344" priority="446" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="329" priority="357" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="343" priority="371" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="328" priority="358" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="342" priority="372" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="327" priority="359" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="341" priority="373" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="326" priority="360" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="340" priority="374" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="325" priority="361" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="339" priority="375" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="324" priority="362" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="338" priority="376" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="323" priority="363" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="337" priority="377" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="322" priority="364" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="336" priority="378" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="321" priority="365" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="335" priority="379" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="containsText" dxfId="320" priority="347" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="334" priority="361" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="319" priority="348" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="333" priority="362" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="318" priority="349" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="332" priority="363" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="317" priority="350" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="331" priority="364" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="316" priority="351" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="330" priority="365" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="315" priority="352" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="329" priority="366" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="314" priority="353" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="328" priority="367" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="313" priority="354" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="327" priority="368" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="312" priority="355" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="326" priority="369" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="311" priority="356" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="325" priority="370" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F16 E45:E57">
-    <cfRule type="containsText" dxfId="310" priority="346" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="324" priority="360" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="309" priority="345" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="323" priority="359" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="308" priority="335" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="322" priority="349" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="307" priority="336" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="321" priority="350" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="306" priority="337" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="320" priority="351" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="305" priority="338" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="319" priority="352" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="304" priority="339" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="318" priority="353" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="303" priority="340" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="317" priority="354" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="302" priority="341" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="316" priority="355" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="301" priority="342" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="315" priority="356" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="300" priority="343" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="314" priority="357" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="299" priority="344" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="313" priority="358" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="298" priority="334" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="312" priority="348" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="297" priority="324" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="311" priority="338" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="296" priority="325" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="310" priority="339" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="295" priority="326" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="309" priority="340" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="294" priority="327" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="308" priority="341" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="293" priority="328" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="307" priority="342" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="292" priority="329" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="306" priority="343" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="291" priority="330" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="305" priority="344" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="290" priority="331" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="304" priority="345" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="289" priority="332" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="303" priority="346" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="288" priority="333" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="302" priority="347" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="containsText" dxfId="287" priority="323" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="301" priority="337" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="286" priority="314" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="300" priority="328" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="285" priority="315" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="299" priority="329" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="284" priority="316" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="298" priority="330" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="283" priority="317" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="297" priority="331" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="282" priority="318" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="296" priority="332" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="281" priority="319" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="295" priority="333" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="280" priority="320" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="294" priority="334" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="279" priority="321" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="293" priority="335" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="278" priority="322" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="292" priority="336" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="277" priority="313" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="291" priority="327" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F26 E45:E57">
-    <cfRule type="containsText" dxfId="276" priority="312" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="290" priority="326" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="275" priority="302" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="289" priority="316" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="274" priority="303" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="288" priority="317" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="304" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="287" priority="318" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="272" priority="305" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="286" priority="319" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="271" priority="306" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="285" priority="320" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="307" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="284" priority="321" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="308" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="283" priority="322" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="268" priority="309" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="282" priority="323" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="267" priority="310" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="281" priority="324" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="266" priority="311" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="280" priority="325" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E26">
-    <cfRule type="containsText" dxfId="265" priority="301" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="279" priority="315" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
+    <cfRule type="containsText" dxfId="278" priority="314" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="277" priority="313" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="276" priority="303" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="275" priority="304" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="274" priority="305" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="273" priority="306" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="272" priority="307" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="271" priority="308" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="270" priority="309" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="269" priority="310" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="268" priority="311" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="267" priority="312" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="266" priority="302" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="containsText" dxfId="265" priority="301" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D29">
     <cfRule type="containsText" dxfId="264" priority="300" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="263" priority="299" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="262" priority="289" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="261" priority="290" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="260" priority="291" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="259" priority="292" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="293" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="294" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="256" priority="295" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="255" priority="296" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="254" priority="297" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="253" priority="298" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="containsText" dxfId="252" priority="288" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="containsText" dxfId="263" priority="291" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="262" priority="292" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="261" priority="293" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="260" priority="294" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="259" priority="295" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="258" priority="296" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="257" priority="297" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="256" priority="298" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="255" priority="299" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="containsText" dxfId="254" priority="290" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="containsText" dxfId="253" priority="289" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="containsText" dxfId="252" priority="288" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
     <cfRule type="containsText" dxfId="251" priority="287" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28:D29">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D33:E33">
     <cfRule type="containsText" dxfId="250" priority="286" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="249" priority="277" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="248" priority="278" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="247" priority="279" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="280" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="281" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="244" priority="282" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="243" priority="283" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="242" priority="284" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="241" priority="285" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="240" priority="276" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="239" priority="275" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="containsText" dxfId="249" priority="276" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="248" priority="277" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="247" priority="278" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="246" priority="279" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="245" priority="280" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="244" priority="281" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="243" priority="282" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="242" priority="283" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="241" priority="284" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="240" priority="285" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="containsText" dxfId="239" priority="275" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31:E31">
     <cfRule type="containsText" dxfId="238" priority="274" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="containsText" dxfId="237" priority="273" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33:E33">
-    <cfRule type="containsText" dxfId="236" priority="272" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="containsText" dxfId="235" priority="262" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="263" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="264" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="232" priority="265" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="231" priority="266" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="267" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="229" priority="268" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="228" priority="269" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="227" priority="270" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="271" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="containsText" dxfId="225" priority="261" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31:E31">
-    <cfRule type="containsText" dxfId="224" priority="260" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" dxfId="223" priority="250" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="237" priority="264" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="251" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="236" priority="265" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="252" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="235" priority="266" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="220" priority="253" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="234" priority="267" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="219" priority="254" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="233" priority="268" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="255" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="232" priority="269" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="256" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="231" priority="270" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="216" priority="257" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="230" priority="271" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="215" priority="258" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="229" priority="272" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="259" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="228" priority="273" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" dxfId="213" priority="249" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="227" priority="263" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
+    <cfRule type="containsText" dxfId="226" priority="262" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:E34">
+    <cfRule type="containsText" dxfId="225" priority="261" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="containsText" dxfId="224" priority="251" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="223" priority="252" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="222" priority="253" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="221" priority="254" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="220" priority="255" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="219" priority="256" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="218" priority="257" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="217" priority="258" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="216" priority="259" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="215" priority="260" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="containsText" dxfId="214" priority="250" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="containsText" dxfId="213" priority="249" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:E35">
     <cfRule type="containsText" dxfId="212" priority="248" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34:E34">
-    <cfRule type="containsText" dxfId="211" priority="247" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="210" priority="237" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="238" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="208" priority="239" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="240" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="241" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="242" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="243" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="203" priority="244" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="245" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="246" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="containsText" dxfId="200" priority="236" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="containsText" dxfId="211" priority="238" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="210" priority="239" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="209" priority="240" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="208" priority="241" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="207" priority="242" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="206" priority="243" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="205" priority="244" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="204" priority="245" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="203" priority="246" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="202" priority="247" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="containsText" dxfId="201" priority="237" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="containsText" dxfId="200" priority="236" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:E36">
     <cfRule type="containsText" dxfId="199" priority="235" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:E35">
-    <cfRule type="containsText" dxfId="198" priority="234" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="197" priority="224" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="225" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="226" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="227" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="228" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="229" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="230" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="231" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="232" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="188" priority="233" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" dxfId="187" priority="223" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="containsText" dxfId="198" priority="225" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="197" priority="226" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="196" priority="227" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="195" priority="228" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="194" priority="229" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="193" priority="230" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="192" priority="231" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="191" priority="232" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="190" priority="233" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="189" priority="234" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="containsText" dxfId="188" priority="224" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="containsText" dxfId="187" priority="215" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="186" priority="216" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="185" priority="217" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="184" priority="218" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="183" priority="219" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="182" priority="220" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="181" priority="221" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="180" priority="222" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="179" priority="223" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="containsText" dxfId="178" priority="214" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:E37">
+    <cfRule type="containsText" dxfId="177" priority="213" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" dxfId="176" priority="203" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="175" priority="204" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="174" priority="205" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="173" priority="206" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="172" priority="207" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="171" priority="208" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="170" priority="209" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="169" priority="210" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="168" priority="211" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="167" priority="212" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" dxfId="166" priority="202" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="containsText" dxfId="165" priority="201" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="containsText" dxfId="164" priority="200" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsText" dxfId="163" priority="199" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsText" dxfId="162" priority="189" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="161" priority="190" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="160" priority="191" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="159" priority="192" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="158" priority="193" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="157" priority="194" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="156" priority="195" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="155" priority="196" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="154" priority="197" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="153" priority="198" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsText" dxfId="152" priority="188" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="containsText" dxfId="151" priority="187" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="containsText" dxfId="150" priority="186" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="containsText" dxfId="149" priority="185" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="containsText" dxfId="148" priority="175" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="147" priority="176" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="146" priority="177" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="145" priority="178" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="144" priority="179" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="143" priority="180" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="142" priority="181" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="141" priority="182" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="140" priority="183" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="139" priority="184" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="containsText" dxfId="138" priority="174" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="containsText" dxfId="137" priority="173" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
+    <cfRule type="containsText" dxfId="136" priority="172" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="135" priority="171" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="134" priority="161" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="133" priority="162" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="132" priority="163" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="131" priority="164" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="130" priority="165" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="129" priority="166" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="128" priority="167" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="127" priority="168" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="126" priority="169" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="125" priority="170" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" dxfId="124" priority="160" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:D44">
+    <cfRule type="containsText" dxfId="123" priority="159" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:D44">
+    <cfRule type="containsText" dxfId="122" priority="158" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="121" priority="157" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="120" priority="147" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="119" priority="148" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="118" priority="149" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="150" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="116" priority="151" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="152" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="153" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="113" priority="154" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="155" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="111" priority="156" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="containsText" dxfId="110" priority="146" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" dxfId="109" priority="145" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" dxfId="108" priority="135" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="107" priority="136" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="106" priority="137" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="138" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="104" priority="139" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="140" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="141" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="101" priority="142" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="143" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="99" priority="144" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" dxfId="98" priority="134" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="containsText" dxfId="97" priority="121" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="containsText" dxfId="96" priority="120" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="186" priority="222" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="95" priority="119" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:E36">
-    <cfRule type="containsText" dxfId="185" priority="221" operator="containsText" text="HIGH">
+  <conditionalFormatting sqref="D36">
+    <cfRule type="containsText" dxfId="94" priority="118" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="184" priority="211" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="212" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="213" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="214" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="215" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="179" priority="216" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="217" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="218" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="176" priority="219" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="220" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" dxfId="174" priority="210" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="173" priority="201" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="202" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="203" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="204" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="205" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="206" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="207" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="208" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="209" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="164" priority="200" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37:E37">
-    <cfRule type="containsText" dxfId="163" priority="199" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" dxfId="162" priority="189" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="190" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="191" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="192" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="193" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="194" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="195" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="155" priority="196" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="197" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="198" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" dxfId="152" priority="188" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="151" priority="187" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="150" priority="186" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="149" priority="185" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="148" priority="175" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="176" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="177" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="178" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="179" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="180" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="181" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="182" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="183" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="184" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="containsText" dxfId="138" priority="174" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="137" priority="173" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="136" priority="172" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="135" priority="171" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="134" priority="161" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="162" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="163" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="164" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="165" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="166" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="167" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="168" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="169" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="170" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" dxfId="124" priority="160" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="containsText" dxfId="123" priority="159" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="containsText" dxfId="122" priority="158" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="121" priority="157" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="120" priority="147" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="148" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="149" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="150" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="151" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="152" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="153" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="154" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="155" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="156" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" dxfId="110" priority="146" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43:D44">
-    <cfRule type="containsText" dxfId="109" priority="145" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43:D44">
-    <cfRule type="containsText" dxfId="108" priority="144" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="107" priority="143" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="106" priority="133" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="134" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="135" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="136" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="137" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="138" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="139" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="140" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="141" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="142" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" dxfId="96" priority="132" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="95" priority="131" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="94" priority="121" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="122" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="123" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="124" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="125" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="126" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="127" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="128" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="129" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="130" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" dxfId="84" priority="120" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="containsText" dxfId="83" priority="107" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="containsText" dxfId="82" priority="106" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="81" priority="105" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="80" priority="104" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="containsText" dxfId="79" priority="103" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="93" priority="117" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="containsText" dxfId="78" priority="102" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="92" priority="116" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="containsText" dxfId="77" priority="101" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="91" priority="115" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="containsText" dxfId="76" priority="100" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="90" priority="114" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
+    <cfRule type="containsText" dxfId="89" priority="113" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="containsText" dxfId="88" priority="112" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="containsText" dxfId="87" priority="111" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57">
+    <cfRule type="containsText" dxfId="86" priority="110" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="85" priority="101" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="84" priority="102" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="83" priority="103" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="82" priority="104" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="81" priority="105" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="80" priority="106" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="79" priority="107" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="78" priority="108" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="109" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="containsText" dxfId="76" priority="100" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
     <cfRule type="containsText" dxfId="75" priority="99" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="containsText" dxfId="74" priority="98" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="containsText" dxfId="73" priority="97" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="containsText" dxfId="72" priority="96" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="71" priority="87" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="88" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="89" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="90" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="91" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="92" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="93" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="94" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="95" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="62" priority="86" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="61" priority="85" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D54)))</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
+    <cfRule type="containsText" dxfId="74" priority="87" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="containsText" dxfId="73" priority="86" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="containsText" dxfId="72" priority="85" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="containsText" dxfId="71" priority="84" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="containsText" dxfId="70" priority="75" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="76" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="77" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="78" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="79" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="80" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="81" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="82" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="83" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="containsText" dxfId="61" priority="74" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
     <cfRule type="containsText" dxfId="60" priority="73" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="59" priority="72" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="58" priority="71" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="57" priority="70" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="56" priority="61" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="62" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="63" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="64" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="65" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="66" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="67" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="68" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="69" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",D39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="47" priority="60" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",D39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="containsText" dxfId="46" priority="59" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D39)))</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="containsText" dxfId="45" priority="38" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="59" priority="52" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="39" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="58" priority="53" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="40" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="57" priority="54" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="41" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="43" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="44" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="53" priority="58" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="45" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="46" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="50" priority="51" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="containsText" dxfId="33" priority="25" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="47" priority="39" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="26" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="46" priority="40" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="27" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="45" priority="41" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="28" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="44" priority="42" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="43" priority="43" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",E46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="42" priority="44" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",E46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="41" priority="45" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="40" priority="46" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",E46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="33" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="39" priority="47" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="34" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="38" priority="48" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",E46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",E46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="36" priority="29" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="35" priority="30" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="33" priority="32" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",D58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",D58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="31" priority="34" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",D58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="22" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="23" operator="containsText" text="OPEN">
+    <cfRule type="containsText" dxfId="28" priority="37" operator="containsText" text="OPEN">
       <formula>NOT(ISERROR(SEARCH("OPEN",D58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="DONE">
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="DONE">
       <formula>NOT(ISERROR(SEARCH("DONE",D58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
+    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="containsText" dxfId="25" priority="17" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="18" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="20" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="26" operator="containsText" text="OPEN">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="DONE">
+      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",E58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
     <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",D58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
+      <formula>NOT(ISERROR(SEARCH("HIGH",D59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
     <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",E59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",E58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",E59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",E58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("LOW",E59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OPEN",E59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HIGH",E59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("DONE",E59)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="OPEN">
-      <formula>NOT(ISERROR(SEARCH("OPEN",E58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
+      <formula>NOT(ISERROR(SEARCH("OPEN",E59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="DONE">
-      <formula>NOT(ISERROR(SEARCH("DONE",E58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
+      <formula>NOT(ISERROR(SEARCH("DONE",E59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",E58)))</formula>
+      <formula>NOT(ISERROR(SEARCH("HIGH",E59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>